<commit_message>
Sprint 1 Meeting 8
</commit_message>
<xml_diff>
--- a/Documents/Sprint One/Sprint_1_Logs.xlsx
+++ b/Documents/Sprint One/Sprint_1_Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B57D992-2CE0-4E9F-8EBA-C85FFFFF818C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D200BE6-9658-4B23-806A-08127C9E9F36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="119">
   <si>
     <t>Question</t>
   </si>
@@ -319,6 +319,75 @@
   </si>
   <si>
     <t>Learned a little about creating more complex page layouts</t>
+  </si>
+  <si>
+    <t>Created/updated layouts for user settings, change password login, forgot, and set security questions pages. Used logos that the team agreed upon in layouts.</t>
+  </si>
+  <si>
+    <t>Looking into intentions and utilizing Google Firebase to control data</t>
+  </si>
+  <si>
+    <t>Nothing unexpected as of yet</t>
+  </si>
+  <si>
+    <t>I worked on the security issue where the user is signed out after 5 minutes of inactivty and the startup page issue and the create account issue, and I created more Mazes for future levels</t>
+  </si>
+  <si>
+    <t>I will work on my assigned issues. Every issue assigned to me will be worked on as well as more level design.</t>
+  </si>
+  <si>
+    <t>No, I am finally working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t>It takes time to get into a good rhythm, but once found, ride it!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I thing that our group should be more on the same page of the design of the app I think we should follow the Model|Presenter|View method for software development. However, we are just sorting hacking issues individually and at the end we are supposidly going to mush all of our work into one project. I am concerned about this getting out of control later on. </t>
+  </si>
+  <si>
+    <t>Completed animation for the sprite for the main character for the Hack Heist app and began work on the user settings button/screen for the in-game menu</t>
+  </si>
+  <si>
+    <t>Continue work on the user settings button/screen for the in-game menu. Begin work on the next sprite for the game.</t>
+  </si>
+  <si>
+    <t>Nothing is currently getting in the way of my work.</t>
+  </si>
+  <si>
+    <t>Currently learning how to make and connect multiple activities in android studio</t>
+  </si>
+  <si>
+    <t>Connecting activities/post spring break I need to spend a lot more time on the project</t>
+  </si>
+  <si>
+    <t>Further work on assigned pages</t>
+  </si>
+  <si>
+    <t>Moved project husk into git repo with several screen layouts finished</t>
+  </si>
+  <si>
+    <t>I have began working on exporting Unity projects to android studio</t>
+  </si>
+  <si>
+    <t>Continue attempting to export projects from Unity to Android studio</t>
+  </si>
+  <si>
+    <t>Currently learning how to modify and build settings on the Unity project</t>
+  </si>
+  <si>
+    <t>No changes currently need to be made to the project due to my work</t>
+  </si>
+  <si>
+    <t>Post spring break I need to spend a lot more time on the project</t>
+  </si>
+  <si>
+    <t>I worked on implementation of the startup page issue and the "create account" issue, and I created more mazes for future levels</t>
+  </si>
+  <si>
+    <t>No, I am working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t>Documentation can really slow down the process of good work, but perhaps has hidden value to be discovered</t>
   </si>
 </sst>
 </file>
@@ -717,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CED5CD-73C7-48F2-87A1-36C83338A6C8}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,13 +864,17 @@
       <c r="G2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>89</v>
       </c>
@@ -820,8 +893,12 @@
       <c r="G3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -845,13 +922,17 @@
       <c r="G4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="97" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -870,8 +951,12 @@
       <c r="G5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -898,8 +983,12 @@
       <c r="G6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -923,8 +1012,12 @@
       <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -948,13 +1041,17 @@
       <c r="G8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -973,8 +1070,12 @@
       <c r="G9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1001,8 +1102,12 @@
       <c r="G10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1026,8 +1131,12 @@
       <c r="G11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1051,8 +1160,12 @@
       <c r="G12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1076,8 +1189,12 @@
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1104,13 +1221,17 @@
       <c r="G14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>89</v>
       </c>
@@ -1129,8 +1250,12 @@
       <c r="G15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1154,8 +1279,12 @@
       <c r="G16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1179,8 +1308,12 @@
       <c r="G17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1207,13 +1340,17 @@
       <c r="G18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="157" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>89</v>
       </c>
@@ -1232,8 +1369,12 @@
       <c r="G19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="H19" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1257,8 +1398,12 @@
       <c r="G20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1282,8 +1427,12 @@
       <c r="G21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>

</xml_diff>

<commit_message>
SPrint 1 Meetin 8 added
</commit_message>
<xml_diff>
--- a/Documents/Sprint One/Sprint_1_Logs.xlsx
+++ b/Documents/Sprint One/Sprint_1_Logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\project-a-group1-imaginationterraformers\Documents\Sprint One\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B57D992-2CE0-4E9F-8EBA-C85FFFFF818C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF08B551-5E3D-4AC6-90E2-6AEBE5436074}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="119">
   <si>
     <t>Question</t>
   </si>
@@ -319,6 +319,75 @@
   </si>
   <si>
     <t>Learned a little about creating more complex page layouts</t>
+  </si>
+  <si>
+    <t>Created/updated layouts for user settings, change password login, forgot, and set security questions pages. Used logos that the team agreed upon in layouts.</t>
+  </si>
+  <si>
+    <t>Moved project husk into git repo with several screen layouts finished</t>
+  </si>
+  <si>
+    <t>I worked on the security issue where the user is signed out after 5 minutes of inactivty and the startup page issue and the create account issue, and I created more Mazes for future levels</t>
+  </si>
+  <si>
+    <t>I worked on implementation of the startup page issue and the "create account" issue, and I created more mazes for future levels</t>
+  </si>
+  <si>
+    <t>Completed animation for the sprite for the main character for the Hack Heist app and began work on the user settings button/screen for the in-game menu</t>
+  </si>
+  <si>
+    <t>I have began working on exporting Unity projects to android studio</t>
+  </si>
+  <si>
+    <t>Looking into intentions and utilizing Google Firebase to control data</t>
+  </si>
+  <si>
+    <t>I will work on my assigned issues. Every issue assigned to me will be worked on as well as more level design.</t>
+  </si>
+  <si>
+    <t>Further work on assigned pages</t>
+  </si>
+  <si>
+    <t>Continue work on the user settings button/screen for the in-game menu. Begin work on the next sprite for the game.</t>
+  </si>
+  <si>
+    <t>Continue attempting to export projects from Unity to Android studio</t>
+  </si>
+  <si>
+    <t>No, I am finally working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t>No, I am working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t>Nothing is currently getting in the way of my work.</t>
+  </si>
+  <si>
+    <t>Nothing unexpected as of yet</t>
+  </si>
+  <si>
+    <t>It takes time to get into a good rhythm, but once found, ride it!</t>
+  </si>
+  <si>
+    <t>Documentation can really slow down the process of good work, but perhaps has hidden value to be discovered</t>
+  </si>
+  <si>
+    <t>Connecting activities/post spring break I need to spend a lot more time on the project</t>
+  </si>
+  <si>
+    <t>Post spring break I need to spend a lot more time on the project</t>
+  </si>
+  <si>
+    <t>Currently learning how to make and connect multiple activities in android studio</t>
+  </si>
+  <si>
+    <t>Currently learning how to modify and build settings on the Unity project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I thing that our group should be more on the same page of the design of the app I think we should follow the Model|Presenter|View method for software development. However, we are just sorting hacking issues individually and at the end we are supposidly going to mush all of our work into one project. I am concerned about this getting out of control later on. </t>
+  </si>
+  <si>
+    <t>No changes currently need to be made to the project due to my work</t>
   </si>
 </sst>
 </file>
@@ -382,12 +451,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -717,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CED5CD-73C7-48F2-87A1-36C83338A6C8}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,13 +810,13 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
@@ -760,16 +828,16 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -777,16 +845,16 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -795,13 +863,17 @@
       <c r="G2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>89</v>
       </c>
@@ -820,8 +892,12 @@
       <c r="G3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -845,8 +921,12 @@
       <c r="G4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -870,8 +950,12 @@
       <c r="G5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -880,7 +964,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -898,8 +982,12 @@
       <c r="G6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -923,8 +1011,12 @@
       <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -948,8 +1040,12 @@
       <c r="G8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -973,8 +1069,12 @@
       <c r="G9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -983,7 +1083,7 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1001,8 +1101,12 @@
       <c r="G10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1026,8 +1130,12 @@
       <c r="G11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1051,8 +1159,12 @@
       <c r="G12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1076,8 +1188,12 @@
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1086,7 +1202,7 @@
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1095,7 +1211,7 @@
       <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1104,8 +1220,12 @@
       <c r="G14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1129,8 +1249,12 @@
       <c r="G15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1154,8 +1278,12 @@
       <c r="G16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1179,8 +1307,12 @@
       <c r="G17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1189,7 +1321,7 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1198,7 +1330,7 @@
       <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1207,8 +1339,12 @@
       <c r="G18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1232,8 +1368,12 @@
       <c r="G19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="H19" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1257,8 +1397,12 @@
       <c r="G20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1282,8 +1426,12 @@
       <c r="G21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>

</xml_diff>

<commit_message>
Sprint 1 Meeting 8 (mistake in last commit, that was meeting 7)
</commit_message>
<xml_diff>
--- a/Documents/Sprint One/Sprint_1_Logs.xlsx
+++ b/Documents/Sprint One/Sprint_1_Logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\project-a-group1-imaginationterraformers\Documents\Sprint One\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF08B551-5E3D-4AC6-90E2-6AEBE5436074}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC5448-BB03-4EA7-8753-4C5A5067F0AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="137">
   <si>
     <t>Question</t>
   </si>
@@ -388,6 +388,60 @@
   </si>
   <si>
     <t>No changes currently need to be made to the project due to my work</t>
+  </si>
+  <si>
+    <t>Got intents working and linked all of the screens I have built thus far. Also renamed layout components in the format of Activity_NameType. This improved the readability in the Java code when mapping java objets to their corrects IDs.</t>
+  </si>
+  <si>
+    <t>Finish planning all topics of discussion for our 'merge meeting', update the github, and continue to look into firebase</t>
+  </si>
+  <si>
+    <t>The use of intentions</t>
+  </si>
+  <si>
+    <t>Changing the format of layout widget names will need to happen at some point to standardize them</t>
+  </si>
+  <si>
+    <t>I worked on the XML and Java file for the main menu, sign up page, and about page.</t>
+  </si>
+  <si>
+    <t>I will work on my assigned issues. Every Issue assigned to me as well as the design and layout of every button and image in all pages for all issues of all assignee.</t>
+  </si>
+  <si>
+    <t>No, I am still working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t>Working together is better than alone!</t>
+  </si>
+  <si>
+    <t>A consistent color scheme/theme will be a necessary addition. However, most likely will not occur until the end of the project</t>
+  </si>
+  <si>
+    <t>Continued attempting to port a Unity project to Android studio</t>
+  </si>
+  <si>
+    <t>Continue looking into porting a Unity project to Android Studio</t>
+  </si>
+  <si>
+    <t>Several errors have prevented me from successfully running a Unity proect in Android Studio</t>
+  </si>
+  <si>
+    <t>Learned more about how to run a Unity project in Andriod Studio</t>
+  </si>
+  <si>
+    <t>No changes currently have to be made to the current plan for the project</t>
+  </si>
+  <si>
+    <t>Created the layout and some functionality for the review page</t>
+  </si>
+  <si>
+    <t>Finish functionality of review, help, and info pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel </t>
+  </si>
+  <si>
+    <t>Learning different ways of adjusting EditText and Ratings</t>
   </si>
 </sst>
 </file>
@@ -785,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CED5CD-73C7-48F2-87A1-36C83338A6C8}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="H18" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -869,7 +923,9 @@
       <c r="I2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
@@ -898,7 +954,9 @@
       <c r="I3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
@@ -927,7 +985,9 @@
       <c r="I4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
@@ -956,7 +1016,9 @@
       <c r="I5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
@@ -988,11 +1050,13 @@
       <c r="I6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="97" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>89</v>
       </c>
@@ -1017,7 +1081,9 @@
       <c r="I7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
@@ -1046,7 +1112,9 @@
       <c r="I8" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
@@ -1075,7 +1143,9 @@
       <c r="I9" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
@@ -1107,7 +1177,9 @@
       <c r="I10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
@@ -1136,7 +1208,9 @@
       <c r="I11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
@@ -1165,7 +1239,9 @@
       <c r="I12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
@@ -1194,7 +1270,9 @@
       <c r="I13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
@@ -1226,7 +1304,9 @@
       <c r="I14" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
@@ -1255,7 +1335,9 @@
       <c r="I15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
@@ -1284,7 +1366,9 @@
       <c r="I16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
@@ -1313,7 +1397,9 @@
       <c r="I17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
@@ -1345,11 +1431,13 @@
       <c r="I18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="82" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>89</v>
       </c>
@@ -1374,7 +1462,9 @@
       <c r="I19" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
@@ -1403,7 +1493,9 @@
       <c r="I20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
@@ -1432,7 +1524,9 @@
       <c r="I21" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added to devinfo and help screens
</commit_message>
<xml_diff>
--- a/Documents/Sprint One/Sprint_1_Logs.xlsx
+++ b/Documents/Sprint One/Sprint_1_Logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\project-a-group1-imaginationterraformers\Documents\Sprint One\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D200BE6-9658-4B23-806A-08127C9E9F36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB5E703-344F-4900-8471-788D74672670}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="146">
   <si>
     <t>Question</t>
   </si>
@@ -388,6 +388,87 @@
   </si>
   <si>
     <t>Documentation can really slow down the process of good work, but perhaps has hidden value to be discovered</t>
+  </si>
+  <si>
+    <t>Got intents working and linked all of the screens I have built thus far. Also renamed layout components in the format of Activity_NameType. This improved the readability in the Java code when mapping java objets to their corrects IDs.</t>
+  </si>
+  <si>
+    <t>I worked on the XML and Java file for the main menu, sign up page, and about page.</t>
+  </si>
+  <si>
+    <t>Created the layout and some functionality for the review page</t>
+  </si>
+  <si>
+    <t>Continued attempting to port a Unity project to Android studio</t>
+  </si>
+  <si>
+    <t>Finish planning all topics of discussion for our 'merge meeting', update the github, and continue to look into firebase</t>
+  </si>
+  <si>
+    <t>I will work on my assigned issues. Every Issue assigned to me as well as the design and layout of every button and image in all pages for all issues of all assignee.</t>
+  </si>
+  <si>
+    <t>Finish functionality of review, help, and info pages</t>
+  </si>
+  <si>
+    <t>Continue looking into porting a Unity project to Android Studio</t>
+  </si>
+  <si>
+    <t>No, I am still working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel </t>
+  </si>
+  <si>
+    <t>Several errors have prevented me from successfully running a Unity proect in Android Studio</t>
+  </si>
+  <si>
+    <t>The use of intentions</t>
+  </si>
+  <si>
+    <t>Working together is better than alone!</t>
+  </si>
+  <si>
+    <t>Learning different ways of adjusting EditText and Ratings</t>
+  </si>
+  <si>
+    <t>Learned more about how to run a Unity project in Andriod Studio</t>
+  </si>
+  <si>
+    <t>Changing the format of layout widget names will need to happen at some point to standardize them</t>
+  </si>
+  <si>
+    <t>A consistent color scheme/theme will be a necessary addition. However, most likely will not occur until the end of the project</t>
+  </si>
+  <si>
+    <t>No changes currently have to be made to the current plan for the project</t>
+  </si>
+  <si>
+    <t>I worked on the intents and Implementation for the main menu, sign up page and about page</t>
+  </si>
+  <si>
+    <t>I will work on my assigned issues. Every issue assigned to me as well as the design and layout of every button and image in all pages for all issues of all assignee.</t>
+  </si>
+  <si>
+    <t>Working together is usually better than alone!</t>
+  </si>
+  <si>
+    <t>Successfully brought a Unity project over to Android studio and ran said project</t>
+  </si>
+  <si>
+    <t>Mapping character movement to UI buttons and integrating the Unity project into a pre-existing Android Studio project</t>
+  </si>
+  <si>
+    <t>Learned how to port a Unity project into Android Studio</t>
+  </si>
+  <si>
+    <t>Finished the current layout for the help page, about page, and review page</t>
+  </si>
+  <si>
+    <t>Continue to work on assigned issues</t>
+  </si>
+  <si>
+    <t>How to use and alter the rating bar and clear them after submission is made</t>
   </si>
 </sst>
 </file>
@@ -456,7 +537,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -468,6 +548,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -786,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CED5CD-73C7-48F2-87A1-36C83338A6C8}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,13 +894,13 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
@@ -829,16 +912,16 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -846,16 +929,16 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -870,7 +953,9 @@
       <c r="I2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
@@ -899,8 +984,12 @@
       <c r="I3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -928,8 +1017,12 @@
       <c r="I4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="97" customHeight="1" x14ac:dyDescent="0.35">
@@ -957,15 +1050,19 @@
       <c r="I5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -989,11 +1086,13 @@
       <c r="I6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>89</v>
       </c>
@@ -1018,8 +1117,12 @@
       <c r="I7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="J7" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1047,8 +1150,12 @@
       <c r="I8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="J8" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1076,15 +1183,19 @@
       <c r="I9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="J9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1108,7 +1219,9 @@
       <c r="I10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
@@ -1137,8 +1250,12 @@
       <c r="I11" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="J11" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1166,8 +1283,12 @@
       <c r="I12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="J12" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1195,15 +1316,19 @@
       <c r="I13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="J13" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1212,7 +1337,7 @@
       <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1227,7 +1352,9 @@
       <c r="I14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
@@ -1256,8 +1383,12 @@
       <c r="I15" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1285,8 +1416,12 @@
       <c r="I16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="J16" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="62" customHeight="1" x14ac:dyDescent="0.35">
@@ -1314,15 +1449,19 @@
       <c r="I17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="J17" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1331,7 +1470,7 @@
       <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1346,7 +1485,9 @@
       <c r="I18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
@@ -1369,14 +1510,18 @@
       <c r="G19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="J19" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -1404,8 +1549,12 @@
       <c r="I20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="J20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
@@ -1433,8 +1582,12 @@
       <c r="I21" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="J21" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="L21" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 1 Meeting 9 added
</commit_message>
<xml_diff>
--- a/Documents/Sprint One/Sprint_1_Logs.xlsx
+++ b/Documents/Sprint One/Sprint_1_Logs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\project-a-group1-imaginationterraformers\Documents\Sprint One\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC5448-BB03-4EA7-8753-4C5A5067F0AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C74403-6958-48FB-8327-41AA4C22A1EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="149">
   <si>
     <t>Question</t>
   </si>
@@ -324,124 +324,160 @@
     <t>Created/updated layouts for user settings, change password login, forgot, and set security questions pages. Used logos that the team agreed upon in layouts.</t>
   </si>
   <si>
+    <t>Looking into intentions and utilizing Google Firebase to control data</t>
+  </si>
+  <si>
+    <t>Nothing unexpected as of yet</t>
+  </si>
+  <si>
+    <t>I worked on the security issue where the user is signed out after 5 minutes of inactivty and the startup page issue and the create account issue, and I created more Mazes for future levels</t>
+  </si>
+  <si>
+    <t>I will work on my assigned issues. Every issue assigned to me will be worked on as well as more level design.</t>
+  </si>
+  <si>
+    <t>No, I am finally working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t>It takes time to get into a good rhythm, but once found, ride it!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I thing that our group should be more on the same page of the design of the app I think we should follow the Model|Presenter|View method for software development. However, we are just sorting hacking issues individually and at the end we are supposidly going to mush all of our work into one project. I am concerned about this getting out of control later on. </t>
+  </si>
+  <si>
+    <t>Completed animation for the sprite for the main character for the Hack Heist app and began work on the user settings button/screen for the in-game menu</t>
+  </si>
+  <si>
+    <t>Continue work on the user settings button/screen for the in-game menu. Begin work on the next sprite for the game.</t>
+  </si>
+  <si>
+    <t>Nothing is currently getting in the way of my work.</t>
+  </si>
+  <si>
+    <t>Currently learning how to make and connect multiple activities in android studio</t>
+  </si>
+  <si>
+    <t>Connecting activities/post spring break I need to spend a lot more time on the project</t>
+  </si>
+  <si>
+    <t>Further work on assigned pages</t>
+  </si>
+  <si>
     <t>Moved project husk into git repo with several screen layouts finished</t>
   </si>
   <si>
-    <t>I worked on the security issue where the user is signed out after 5 minutes of inactivty and the startup page issue and the create account issue, and I created more Mazes for future levels</t>
+    <t>I have began working on exporting Unity projects to android studio</t>
+  </si>
+  <si>
+    <t>Continue attempting to export projects from Unity to Android studio</t>
+  </si>
+  <si>
+    <t>Currently learning how to modify and build settings on the Unity project</t>
+  </si>
+  <si>
+    <t>No changes currently need to be made to the project due to my work</t>
+  </si>
+  <si>
+    <t>Post spring break I need to spend a lot more time on the project</t>
   </si>
   <si>
     <t>I worked on implementation of the startup page issue and the "create account" issue, and I created more mazes for future levels</t>
   </si>
   <si>
-    <t>Completed animation for the sprite for the main character for the Hack Heist app and began work on the user settings button/screen for the in-game menu</t>
-  </si>
-  <si>
-    <t>I have began working on exporting Unity projects to android studio</t>
-  </si>
-  <si>
-    <t>Looking into intentions and utilizing Google Firebase to control data</t>
-  </si>
-  <si>
-    <t>I will work on my assigned issues. Every issue assigned to me will be worked on as well as more level design.</t>
-  </si>
-  <si>
-    <t>Further work on assigned pages</t>
-  </si>
-  <si>
-    <t>Continue work on the user settings button/screen for the in-game menu. Begin work on the next sprite for the game.</t>
-  </si>
-  <si>
-    <t>Continue attempting to export projects from Unity to Android studio</t>
-  </si>
-  <si>
-    <t>No, I am finally working with all cylinders pumping</t>
-  </si>
-  <si>
     <t>No, I am working with all cylinders pumping</t>
   </si>
   <si>
-    <t>Nothing is currently getting in the way of my work.</t>
-  </si>
-  <si>
-    <t>Nothing unexpected as of yet</t>
-  </si>
-  <si>
-    <t>It takes time to get into a good rhythm, but once found, ride it!</t>
-  </si>
-  <si>
     <t>Documentation can really slow down the process of good work, but perhaps has hidden value to be discovered</t>
   </si>
   <si>
-    <t>Connecting activities/post spring break I need to spend a lot more time on the project</t>
-  </si>
-  <si>
-    <t>Post spring break I need to spend a lot more time on the project</t>
-  </si>
-  <si>
-    <t>Currently learning how to make and connect multiple activities in android studio</t>
-  </si>
-  <si>
-    <t>Currently learning how to modify and build settings on the Unity project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I thing that our group should be more on the same page of the design of the app I think we should follow the Model|Presenter|View method for software development. However, we are just sorting hacking issues individually and at the end we are supposidly going to mush all of our work into one project. I am concerned about this getting out of control later on. </t>
-  </si>
-  <si>
-    <t>No changes currently need to be made to the project due to my work</t>
-  </si>
-  <si>
     <t>Got intents working and linked all of the screens I have built thus far. Also renamed layout components in the format of Activity_NameType. This improved the readability in the Java code when mapping java objets to their corrects IDs.</t>
   </si>
   <si>
+    <t>I worked on the XML and Java file for the main menu, sign up page, and about page.</t>
+  </si>
+  <si>
+    <t>I worked on intents and implementation for the main menu, sign up page,e and about page.</t>
+  </si>
+  <si>
+    <t>Created the layout and some functionality for the review page</t>
+  </si>
+  <si>
+    <t>Finished the review page and help page</t>
+  </si>
+  <si>
+    <t>Continued attempting to port a Unity project to Android studio</t>
+  </si>
+  <si>
+    <t>Successfully brought a Unity project over to Android studio and ran said project</t>
+  </si>
+  <si>
     <t>Finish planning all topics of discussion for our 'merge meeting', update the github, and continue to look into firebase</t>
   </si>
   <si>
+    <t>I will work on my assigned issues. Every Issue assigned to me as well as the design and layout of every button and image in all pages for all issues of all assignee.</t>
+  </si>
+  <si>
+    <t>Finish functionality of review, help, and info pages</t>
+  </si>
+  <si>
+    <t>Figure out mail gun for sending emails to the developers</t>
+  </si>
+  <si>
+    <t>Continue looking into porting a Unity project to Android Studio</t>
+  </si>
+  <si>
+    <t>Mapping character movement to UI buttons and integrating the Unity project into an existing Android studio project</t>
+  </si>
+  <si>
+    <t>No, I am still working with all cylinders pumping</t>
+  </si>
+  <si>
+    <t>No, I am always working with all cylindrs pumping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel </t>
+  </si>
+  <si>
+    <t>Several errors have prevented me from successfully running a Unity proect in Android Studio</t>
+  </si>
+  <si>
     <t>The use of intentions</t>
   </si>
   <si>
+    <t>Working together is better than alone!</t>
+  </si>
+  <si>
+    <t>Learning different ways of adjusting EditText and Ratings</t>
+  </si>
+  <si>
+    <t>Team work is valuable and communication is key in order to save time</t>
+  </si>
+  <si>
+    <t>Learned more about how to run a Unity project in Andriod Studio</t>
+  </si>
+  <si>
+    <t>Learned how to port a Unity project into Android studio</t>
+  </si>
+  <si>
     <t>Changing the format of layout widget names will need to happen at some point to standardize them</t>
   </si>
   <si>
-    <t>I worked on the XML and Java file for the main menu, sign up page, and about page.</t>
-  </si>
-  <si>
-    <t>I will work on my assigned issues. Every Issue assigned to me as well as the design and layout of every button and image in all pages for all issues of all assignee.</t>
-  </si>
-  <si>
-    <t>No, I am still working with all cylinders pumping</t>
-  </si>
-  <si>
-    <t>Working together is better than alone!</t>
-  </si>
-  <si>
     <t>A consistent color scheme/theme will be a necessary addition. However, most likely will not occur until the end of the project</t>
   </si>
   <si>
-    <t>Continued attempting to port a Unity project to Android studio</t>
-  </si>
-  <si>
-    <t>Continue looking into porting a Unity project to Android Studio</t>
-  </si>
-  <si>
-    <t>Several errors have prevented me from successfully running a Unity proect in Android Studio</t>
-  </si>
-  <si>
-    <t>Learned more about how to run a Unity project in Andriod Studio</t>
-  </si>
-  <si>
     <t>No changes currently have to be made to the current plan for the project</t>
   </si>
   <si>
-    <t>Created the layout and some functionality for the review page</t>
-  </si>
-  <si>
-    <t>Finish functionality of review, help, and info pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel </t>
-  </si>
-  <si>
-    <t>Learning different ways of adjusting EditText and Ratings</t>
+    <t>Built application data validation for screens. Minor layout tweaks. Firebase updates.</t>
+  </si>
+  <si>
+    <t>Continue to look into firebase</t>
+  </si>
+  <si>
+    <t>Difficulty reading/writing to firebase</t>
+  </si>
+  <si>
+    <t>Establishing a connection to firebase</t>
   </si>
 </sst>
 </file>
@@ -839,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CED5CD-73C7-48F2-87A1-36C83338A6C8}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H18" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,15 +957,17 @@
         <v>96</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>89</v>
       </c>
@@ -949,15 +987,17 @@
         <v>72</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -986,12 +1026,14 @@
         <v>68</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K4" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="97" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1011,15 +1053,17 @@
         <v>76</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K5" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1045,18 +1089,20 @@
         <v>80</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K6" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="97" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>89</v>
       </c>
@@ -1076,15 +1122,17 @@
         <v>73</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1107,18 +1155,20 @@
         <v>86</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K8" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1141,12 +1191,14 @@
         <v>105</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="74" customHeight="1" x14ac:dyDescent="0.35">
@@ -1180,7 +1232,9 @@
       <c r="J10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -1203,15 +1257,17 @@
         <v>74</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K11" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1240,9 +1296,11 @@
         <v>82</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="K12" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1265,15 +1323,17 @@
         <v>32</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -1299,18 +1359,20 @@
         <v>81</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K14" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>89</v>
       </c>
@@ -1330,15 +1392,17 @@
         <v>75</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K15" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1361,15 +1425,17 @@
         <v>83</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K16" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="62" customHeight="1" x14ac:dyDescent="0.35">
@@ -1392,15 +1458,17 @@
         <v>78</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K17" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1432,12 +1500,14 @@
         <v>24</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K18" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="82" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="157" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>89</v>
       </c>
@@ -1457,15 +1527,17 @@
         <v>52</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K19" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -1496,7 +1568,9 @@
       <c r="J20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
@@ -1519,15 +1593,17 @@
         <v>64</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K21" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="L21" s="1"/>
     </row>
   </sheetData>

</xml_diff>